<commit_message>
Changes at GUI/Database... and testing classes.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="15">
   <si>
     <t>Παραδόσεις 24-05-2016</t>
   </si>
@@ -66,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00 €"/>
   </numFmts>
-  <fonts count="91">
+  <fonts count="98">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -87,6 +87,39 @@
     <font>
       <name val="Calibri"/>
       <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="20.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="16.0"/>
       <b val="true"/>
     </font>
     <font>
@@ -641,7 +674,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="268">
+  <cellXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="bottom"/>
@@ -1064,6 +1097,43 @@
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1078,72 +1148,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.41796875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.8125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.7265625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.80078125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="14.33984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.58203125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="16.5234375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.59765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="243">
+      <c r="A1" t="s" s="268">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="244">
+      <c r="A2" t="s" s="269">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="246">
+      <c r="A3" t="s" s="271">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n" s="272">
+        <v>34.12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="274">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n" s="275">
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="277">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n" s="278">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="280">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n" s="281">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="283">
+        <v>3</v>
+      </c>
+      <c r="B7" t="n" s="284">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="286">
         <v>2</v>
       </c>
-      <c r="B3" t="n" s="247">
+      <c r="B8" t="n" s="287">
         <v>22.0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s" s="249">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n" s="250">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="252">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n" s="253">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="255">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n" s="256">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="258">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n" s="259">
-        <v>34.12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="261">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n" s="262">
-        <v>12.45</v>
-      </c>
-    </row>
     <row r="9">
-      <c r="A9" t="s" s="263">
+      <c r="A9" t="s" s="288">
         <v>8</v>
       </c>
     </row>
@@ -1174,16 +1244,16 @@
     </row>
     <row r="44" ht="20.0" customHeight="true"/>
     <row r="46">
-      <c r="A46" t="s" s="264">
+      <c r="A46" t="s" s="289">
         <v>12</v>
       </c>
-      <c r="B46" t="n" s="265">
+      <c r="B46" t="n" s="290">
         <v>136.47</v>
       </c>
-      <c r="C46" t="s" s="266">
+      <c r="C46" t="s" s="291">
         <v>13</v>
       </c>
-      <c r="D46" t="s" s="267">
+      <c r="D46" t="s" s="292">
         <v>14</v>
       </c>
     </row>

</xml_diff>